<commit_message>
Removed kart pivot table as redundant
</commit_message>
<xml_diff>
--- a/data/processed/Manual times.xlsx
+++ b/data/processed/Manual times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arcelormittal-my.sharepoint.com/personal/jeremy_walsh_arcelormittal_com/Documents/Documents/GitHub/GoKarts/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="8_{9203E252-FD71-414A-9075-16F581A28679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF7BCF9B-2957-4409-9157-0C8CEB9C8EB9}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="8_{9203E252-FD71-414A-9075-16F581A28679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EAC7B09-900A-4AAB-B4E4-080FCCF19054}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B8025F23-8904-4793-8FB4-5451A531D2DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B8025F23-8904-4793-8FB4-5451A531D2DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Race 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Race 3" sheetId="5" r:id="rId3"/>
     <sheet name="Race 4" sheetId="6" r:id="rId4"/>
     <sheet name="Karts" sheetId="7" r:id="rId5"/>
-    <sheet name="Karts Pivot" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
   <si>
     <t>Lap</t>
   </si>
@@ -66,15 +65,6 @@
   </si>
   <si>
     <t>Race</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Race Number</t>
-  </si>
-  <si>
-    <t>Kart Number</t>
   </si>
 </sst>
 </file>
@@ -148,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -160,9 +150,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -481,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBD5726-9B87-4D31-A6AF-49F9D4A7FBCF}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4728,8 +4715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA36D72B-46E8-4EAD-BF9E-542149F04A9D}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4818,7 +4805,7 @@
         <v>25</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4844,7 +4831,7 @@
         <v>21</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4877,338 +4864,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9B02D0-CDB1-4056-8DF7-B1F1BBA6BC00}">
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>19</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>25</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>21</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>10</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>19</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>6</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>